<commit_message>
automatic excel coverage writer/coordinates/distance matrix
</commit_message>
<xml_diff>
--- a/clusters_with_coordinates.xlsx
+++ b/clusters_with_coordinates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhammed Karakurt\Desktop\IE 492 Final Project\Codes\IE492-HEURISTICS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhammed Karakurt\Desktop\IE 492 Final Project\Codes\IE492-GLOBAL SCORES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CC22DC-B4DF-4CEE-9842-CD6857E3AE39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA841A5-B896-41E2-B97D-EEE507A82B02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -673,7 +673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>